<commit_message>
setting initial negative keywords
</commit_message>
<xml_diff>
--- a/negatives.xlsx
+++ b/negatives.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="21000" windowHeight="10020"/>
+    <workbookView windowWidth="28785" windowHeight="10620"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,12 +27,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Negative</t>
   </si>
   <si>
     <t>sex</t>
+  </si>
+  <si>
+    <t>shit</t>
+  </si>
+  <si>
+    <t>fuck</t>
   </si>
 </sst>
 </file>
@@ -967,13 +973,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="E5" sqref="E5:F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="1"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="3"/>
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
@@ -985,6 +991,16 @@
         <v>1</v>
       </c>
     </row>
+    <row r="3" spans="1:1">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>

</xml_diff>